<commit_message>
Agregado el flujo 3
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -5,7 +5,8 @@
   <sheets>
     <sheet state="visible" name="url" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="productos" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Hoja 3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="validarCat" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="validarHome" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nombres</t>
   </si>
@@ -30,61 +31,46 @@
     <t>keyword</t>
   </si>
   <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
     <t>calavera</t>
   </si>
   <si>
-    <t>//a[@href='https://zippo.com.co/product/encendedor-zippo-calavera-naipe/']</t>
-  </si>
-  <si>
-    <t>//h2[contains(text(),'Encendedor Zippo Calavera Naipe')]</t>
-  </si>
-  <si>
     <t>dragon</t>
   </si>
   <si>
-    <t>//a[@href='https://zippo.com.co/product/encededor-zippo-dragon-ace-29840/']</t>
-  </si>
-  <si>
-    <t>//h2[contains(text(),'Encededor Zippo Dragon Ace')]</t>
-  </si>
-  <si>
     <t>estuche</t>
   </si>
   <si>
-    <t>//a[@href='https://zippo.com.co/product/lplbk-estuche-zippo-cuero-negro-correa/']</t>
-  </si>
-  <si>
-    <t>//h2[contains(text(),'Lplbk Estuche Zippo Cuero Negro/correa')]</t>
-  </si>
-  <si>
     <t>electrico</t>
   </si>
   <si>
-    <t>Paso a paso Flujo 1</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>buscar barra de busqueda</t>
-  </si>
-  <si>
-    <t>//input[@id='woocommerce-product-search-field-0']</t>
-  </si>
-  <si>
-    <t>escribir texto y dar enter</t>
-  </si>
-  <si>
-    <t>buscar elemento</t>
-  </si>
-  <si>
-    <t>verificar que el nombre de la pagina corresponda con el elemento</t>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Encendedor Zippo Calavera Naipe</t>
+  </si>
+  <si>
+    <t>Estuche Zippo Cuero Cafe / Correa – Cod Lplb</t>
+  </si>
+  <si>
+    <t>Inserto Zippo Llama Amarilla</t>
+  </si>
+  <si>
+    <t>Texto</t>
+  </si>
+  <si>
+    <t>Combustible Para Encendedor Zippo 4oz – Cod 3141laex</t>
+  </si>
+  <si>
+    <t>Dispensador Guarda Combustible Zippo – Cod 121503</t>
+  </si>
+  <si>
+    <t>Inserto Encendedor Zippo Butano Llama Sencilla Cod 65826</t>
+  </si>
+  <si>
+    <t>Inserto Encendedor Zippo Butano Llama Doble Cod 65827</t>
+  </si>
+  <si>
+    <t>Mecha Para Encendedor Zippo – Cod 2425</t>
   </si>
 </sst>
 </file>
@@ -108,12 +94,18 @@
       <color rgb="FF1155CC"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -132,6 +124,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -149,6 +144,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -402,49 +401,25 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -462,61 +437,74 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="2.88"/>
+    <col customWidth="1" min="1" max="1" width="26.63"/>
     <col customWidth="1" min="2" max="2" width="49.5"/>
     <col customWidth="1" min="3" max="3" width="38.63"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>